<commit_message>
Changed trainers.xlsx for testing
</commit_message>
<xml_diff>
--- a/trainers.xlsx
+++ b/trainers.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6090"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sample Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -30,40 +28,64 @@
     <t>Email</t>
   </si>
   <si>
+    <t>9876543210</t>
+  </si>
+  <si>
+    <t>Ted Mosby</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>vaishnavipatil10march@gmail.com</t>
+  </si>
+  <si>
+    <t>Sheldon Cooper</t>
+  </si>
+  <si>
     <t>L&amp;D</t>
   </si>
   <si>
-    <t>Ted Mosby</t>
-  </si>
-  <si>
-    <t>R&amp;D</t>
-  </si>
-  <si>
-    <t>Sheldon Cooper</t>
-  </si>
-  <si>
-    <t>put your email here</t>
+    <t>vaishnavi10march2000@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="48"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,18 +97,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -385,81 +410,62 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>9876456723</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>9835672893</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>